<commit_message>
git commit -m 'update code'
</commit_message>
<xml_diff>
--- a/CIS eFAS Industry DB Scraping/IT_EFAS_INDU_COMMON_DB/COMMON_DB/additionalExportImport.xlsx
+++ b/CIS eFAS Industry DB Scraping/IT_EFAS_INDU_COMMON_DB/COMMON_DB/additionalExportImport.xlsx
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E2" t="n">
-        <v>673</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3848</v>
+        <v>4422</v>
       </c>
       <c r="E3" t="n">
-        <v>8682</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -523,16 +523,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6231</v>
+        <v>5491</v>
       </c>
       <c r="E4" t="n">
-        <v>3249</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -546,16 +546,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2064</v>
+        <v>1378</v>
       </c>
       <c r="E5" t="n">
-        <v>1374</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -569,16 +569,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>729</v>
+        <v>576</v>
       </c>
       <c r="E6" t="n">
-        <v>1007</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -592,16 +592,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="E7" t="n">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -615,16 +615,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1120</v>
+        <v>822</v>
       </c>
       <c r="E8" t="n">
-        <v>689</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -638,16 +638,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="E9" t="n">
-        <v>246</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -661,16 +661,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E10" t="n">
-        <v>185</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" t="n">
         <v>19</v>
@@ -693,7 +693,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -707,16 +707,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1919</v>
+        <v>1240</v>
       </c>
       <c r="E12" t="n">
-        <v>388</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -730,16 +730,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3095</v>
+        <v>2254</v>
       </c>
       <c r="E13" t="n">
-        <v>1371</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -753,16 +753,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1443</v>
+        <v>1126</v>
       </c>
       <c r="E14" t="n">
-        <v>2009</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -776,16 +776,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="E15" t="n">
-        <v>142</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -799,16 +799,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1212</v>
+        <v>1108</v>
       </c>
       <c r="E16" t="n">
-        <v>863</v>
+        <v>867</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -822,16 +822,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>10823</v>
+        <v>6099</v>
       </c>
       <c r="E17" t="n">
-        <v>5745</v>
+        <v>5141</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -845,16 +845,16 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>470</v>
+        <v>1043</v>
       </c>
       <c r="E18" t="n">
-        <v>295</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -868,16 +868,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>719</v>
+        <v>569</v>
       </c>
       <c r="E19" t="n">
-        <v>556</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -891,16 +891,16 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="E20" t="n">
-        <v>1321</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -914,16 +914,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>709</v>
+        <v>655</v>
       </c>
       <c r="E21" t="n">
-        <v>2882</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -937,16 +937,16 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>957</v>
+        <v>728</v>
       </c>
       <c r="E22" t="n">
-        <v>985</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -960,16 +960,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1575</v>
+        <v>628</v>
       </c>
       <c r="E23" t="n">
-        <v>996</v>
+        <v>863</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1490</v>
+        <v>1256</v>
       </c>
       <c r="E24" t="n">
-        <v>1834</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1006,16 +1006,16 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1329</v>
+        <v>1212</v>
       </c>
       <c r="E25" t="n">
-        <v>1339</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1029,16 +1029,16 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>734</v>
+        <v>811</v>
       </c>
       <c r="E26" t="n">
-        <v>395</v>
+        <v>828</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1052,16 +1052,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2247</v>
+        <v>2068</v>
       </c>
       <c r="E27" t="n">
-        <v>1516</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1075,16 +1075,16 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2566</v>
+        <v>2028</v>
       </c>
       <c r="E28" t="n">
-        <v>2164</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1098,16 +1098,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6294</v>
+        <v>6824</v>
       </c>
       <c r="E29" t="n">
-        <v>1549</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1121,16 +1121,16 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>695</v>
+        <v>1356</v>
       </c>
       <c r="E30" t="n">
-        <v>350</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1144,16 +1144,16 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>906</v>
+        <v>638</v>
       </c>
       <c r="E31" t="n">
-        <v>583</v>
+        <v>443</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1167,16 +1167,16 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="E32" t="n">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1190,16 +1190,16 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="E33" t="n">
-        <v>569</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1213,16 +1213,16 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="E34" t="n">
-        <v>1054</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1236,16 +1236,16 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E35" t="n">
-        <v>751</v>
+        <v>766</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1262,13 +1262,13 @@
         <v>5</v>
       </c>
       <c r="E36" t="n">
-        <v>313</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1282,16 +1282,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E37" t="n">
-        <v>322</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>202201</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1305,10 +1305,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E38" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>